<commit_message>
Added placeholder confience column with default values of 'unknown'
</commit_message>
<xml_diff>
--- a/events/events.xlsx
+++ b/events/events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\git\ids-simulator-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laymanl\git\ids-simulator-analysis\events\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90369B46-9011-480E-9A64-413E30FC1CBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3868B376-7FBA-4629-AE00-43667E5CCDDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="63">
   <si>
     <t>should_escalate</t>
   </si>
@@ -219,6 +221,12 @@
   </si>
   <si>
     <t>scenario</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>confidence</t>
   </si>
 </sst>
 </file>
@@ -7080,10 +7088,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7103,7 +7111,7 @@
     <col min="13" max="1021" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -7143,8 +7151,11 @@
       <c r="M1" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7185,8 +7196,11 @@
       <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7227,8 +7241,11 @@
       <c r="M3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7269,8 +7286,11 @@
       <c r="M4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7311,8 +7331,11 @@
       <c r="M5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7353,8 +7376,11 @@
       <c r="M6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7395,8 +7421,11 @@
       <c r="M7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7437,8 +7466,11 @@
       <c r="M8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -7479,8 +7511,11 @@
       <c r="M9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7521,8 +7556,11 @@
       <c r="M10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -7563,8 +7601,11 @@
       <c r="M11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -7605,8 +7646,11 @@
       <c r="M12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -7647,8 +7691,11 @@
       <c r="M13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -7689,8 +7736,11 @@
       <c r="M14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -7731,8 +7781,11 @@
       <c r="M15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -7773,8 +7826,11 @@
       <c r="M16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -7815,8 +7871,11 @@
       <c r="M17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -7857,8 +7916,11 @@
       <c r="M18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -7899,8 +7961,11 @@
       <c r="M19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -7941,8 +8006,11 @@
       <c r="M20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -7983,8 +8051,11 @@
       <c r="M21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8025,8 +8096,11 @@
       <c r="M22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -8067,8 +8141,11 @@
       <c r="M23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -8109,8 +8186,11 @@
       <c r="M24" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -8151,8 +8231,11 @@
       <c r="M25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -8193,8 +8276,11 @@
       <c r="M26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -8235,8 +8321,11 @@
       <c r="M27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -8277,8 +8366,11 @@
       <c r="M28" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -8319,8 +8411,11 @@
       <c r="M29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -8361,8 +8456,11 @@
       <c r="M30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -8403,8 +8501,11 @@
       <c r="M31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -8445,8 +8546,11 @@
       <c r="M32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -8487,8 +8591,11 @@
       <c r="M33" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -8529,8 +8636,11 @@
       <c r="M34" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -8571,8 +8681,11 @@
       <c r="M35" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -8613,8 +8726,11 @@
       <c r="M36" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -8655,8 +8771,11 @@
       <c r="M37" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -8697,8 +8816,11 @@
       <c r="M38" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -8739,8 +8861,11 @@
       <c r="M39" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -8781,8 +8906,11 @@
       <c r="M40" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -8823,8 +8951,11 @@
       <c r="M41" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -8865,8 +8996,11 @@
       <c r="M42" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -8907,8 +9041,11 @@
       <c r="M43" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -8949,8 +9086,11 @@
       <c r="M44" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -8991,8 +9131,11 @@
       <c r="M45" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -9033,8 +9176,11 @@
       <c r="M46" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -9075,8 +9221,11 @@
       <c r="M47" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -9117,8 +9266,11 @@
       <c r="M48" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -9159,8 +9311,11 @@
       <c r="M49" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -9201,8 +9356,11 @@
       <c r="M50" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -9243,8 +9401,11 @@
       <c r="M51" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -9285,8 +9446,11 @@
       <c r="M52" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -9327,8 +9491,11 @@
       <c r="M53" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -9369,8 +9536,11 @@
       <c r="M54" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -9411,8 +9581,11 @@
       <c r="M55" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -9453,8 +9626,11 @@
       <c r="M56" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -9495,8 +9671,11 @@
       <c r="M57" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -9537,8 +9716,11 @@
       <c r="M58" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -9579,8 +9761,11 @@
       <c r="M59" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -9621,8 +9806,11 @@
       <c r="M60" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N60" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -9663,8 +9851,11 @@
       <c r="M61" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -9705,8 +9896,11 @@
       <c r="M62" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -9747,8 +9941,11 @@
       <c r="M63" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -9789,8 +9986,11 @@
       <c r="M64" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N64" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -9831,8 +10031,11 @@
       <c r="M65" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N65" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -9873,8 +10076,11 @@
       <c r="M66" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N66" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -9915,8 +10121,11 @@
       <c r="M67" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -9957,8 +10166,11 @@
       <c r="M68" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N68" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -9999,8 +10211,11 @@
       <c r="M69" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -10041,8 +10256,11 @@
       <c r="M70" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N70" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -10083,8 +10301,11 @@
       <c r="M71" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -10125,8 +10346,11 @@
       <c r="M72" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N72" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -10167,8 +10391,11 @@
       <c r="M73" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N73" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -10208,6 +10435,9 @@
       </c>
       <c r="M74" t="s">
         <v>40</v>
+      </c>
+      <c r="N74" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>